<commit_message>
FA-1991 & FA 1992 Done
</commit_message>
<xml_diff>
--- a/datafiles/businessReportData.xlsx
+++ b/datafiles/businessReportData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25721"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/IdeaProjects/FalconMain/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975DDE71-B40C-9C4A-889D-E81F2F6ED96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{418C4432-9F7E-4515-8571-E19C80D628B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="10920" windowWidth="14800" windowHeight="8020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10080" yWindow="10920" windowWidth="14800" windowHeight="8020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,6 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
+    <t>reportType</t>
+  </si>
+  <si>
     <t>exDay</t>
   </si>
   <si>
@@ -50,16 +57,13 @@
     <t>exYear2</t>
   </si>
   <si>
+    <t>searchData</t>
+  </si>
+  <si>
+    <t>reportFilter</t>
+  </si>
+  <si>
     <t>Users Details</t>
-  </si>
-  <si>
-    <t>reportFilter</t>
-  </si>
-  <si>
-    <t>searchData</t>
-  </si>
-  <si>
-    <t>reportType</t>
   </si>
   <si>
     <t>MAR</t>
@@ -458,47 +462,47 @@
       <selection activeCell="B2" sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -548,40 +552,40 @@
       <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>2</v>

</xml_diff>